<commit_message>
add validators, add goods, fix range slider, change error handler
</commit_message>
<xml_diff>
--- a/SunnyFlamingo/newGoods.xlsx
+++ b/SunnyFlamingo/newGoods.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -31,18 +31,18 @@
     <t>ProducerId</t>
   </si>
   <si>
+    <t>MaterialValue</t>
+  </si>
+  <si>
+    <t>ColorValue</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
     <t>ManufacturerId</t>
   </si>
   <si>
-    <t>MaterialValue</t>
-  </si>
-  <si>
-    <t>ColorValue</t>
-  </si>
-  <si>
-    <t>UserId</t>
-  </si>
-  <si>
     <t>Discriminator</t>
   </si>
   <si>
@@ -148,10 +148,10 @@
     <t>AMD</t>
   </si>
   <si>
-    <t>Gbfgbfgb</t>
-  </si>
-  <si>
-    <t>dfdbfgbsfb</t>
+    <t>dfdbfgb</t>
+  </si>
+  <si>
+    <t>Fdgfbfgb</t>
   </si>
 </sst>
 </file>
@@ -498,15 +498,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM2"/>
+  <dimension ref="A1:AM20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.6640625" customWidth="1"/>
+    <col min="22" max="22" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.44140625" customWidth="1"/>
+    <col min="30" max="30" width="8.21875" customWidth="1"/>
+    <col min="31" max="31" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.3">
@@ -526,16 +564,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
       </c>
       <c r="J1" t="s">
         <v>9</v>
@@ -630,16 +668,16 @@
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1">
-        <v>9789744.3200000003</v>
+        <v>23344.32</v>
       </c>
       <c r="C2" t="s">
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>40</v>
@@ -651,19 +689,19 @@
         <v>42</v>
       </c>
       <c r="K2" s="2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="2">
         <v>8</v>
       </c>
-      <c r="L2" s="2">
-        <v>16</v>
-      </c>
       <c r="M2" s="2">
-        <v>34</v>
+        <v>4</v>
       </c>
       <c r="N2" s="2">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="O2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P2" t="s">
         <v>39</v>
@@ -685,7 +723,242 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="AM3" s="2"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="AM4" s="2"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="AM5" s="2"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="AM6" s="2"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="AM7" s="2"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+      <c r="AM8" s="2"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="AM9" s="2"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="AM10" s="2"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="AM11" s="2"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="AM12" s="2"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="AM13" s="2"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="AM14" s="2"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+      <c r="AM15" s="2"/>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="AM16" s="2"/>
+    </row>
+    <row r="17" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="AM17" s="2"/>
+    </row>
+    <row r="18" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="AM18" s="2"/>
+    </row>
+    <row r="19" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="AM19" s="2"/>
+    </row>
+    <row r="20" spans="2:39" x14ac:dyDescent="0.3">
+      <c r="B20" s="1"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="AM20" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>